<commit_message>
Added option to generate L3A with all resampled bands (10m and 20m)
</commit_message>
<xml_diff>
--- a/sen2agri-processors/Composite/Docs/ConcatenatedInputRaster.xlsx
+++ b/sen2agri-processors/Composite/Docs/ConcatenatedInputRaster.xlsx
@@ -9,18 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985" tabRatio="254"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985" tabRatio="327"/>
   </bookViews>
   <sheets>
     <sheet name="Resolution 10" sheetId="1" r:id="rId1"/>
     <sheet name="Resolution 20" sheetId="2" r:id="rId2"/>
+    <sheet name="AllInOne" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="61">
   <si>
     <t>Concatenated Input Raster</t>
   </si>
@@ -167,6 +168,42 @@
   </si>
   <si>
     <t>Spot4 Index</t>
+  </si>
+  <si>
+    <t>Pixel status L3A</t>
+  </si>
+  <si>
+    <t>Weighted Average Ref B12 L3A</t>
+  </si>
+  <si>
+    <t>Weighted Average Ref B11 L3A</t>
+  </si>
+  <si>
+    <t>Weighted Average Ref B2 L3A</t>
+  </si>
+  <si>
+    <t>Weighted Average Ref B3 L3A</t>
+  </si>
+  <si>
+    <t>Weighted Average Ref B4 L3A</t>
+  </si>
+  <si>
+    <t>Weighted Average Ref B8 L3A</t>
+  </si>
+  <si>
+    <t>Weighted Average Ref B5 L3A</t>
+  </si>
+  <si>
+    <t>Weighted Average Ref B6 L3A</t>
+  </si>
+  <si>
+    <t>Weighted Average Ref B7 L3A</t>
+  </si>
+  <si>
+    <t>Weighted Average Ref B8A L3A</t>
+  </si>
+  <si>
+    <t>YES</t>
   </si>
 </sst>
 </file>
@@ -213,7 +250,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -226,6 +263,15 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -512,7 +558,7 @@
   <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20:G20"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -524,11 +570,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -892,95 +938,194 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+    </row>
+    <row r="25" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B25" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E25" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>1</v>
+        <f>A25+1</f>
+        <v>2</v>
       </c>
       <c r="B26" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="1">
-        <v>2</v>
+      <c r="E26" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A27" s="5">
+        <f t="shared" ref="A27:A34" si="2">A26+1</f>
+        <v>3</v>
       </c>
       <c r="B27" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="1">
-        <v>3</v>
+      <c r="E27" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A28" s="5">
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
       <c r="B28" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="1">
-        <v>4</v>
+      <c r="E28" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A29" s="5">
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="B29" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="1">
-        <v>5</v>
+      <c r="E29" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A30" s="5">
+        <f t="shared" si="2"/>
+        <v>6</v>
       </c>
       <c r="B30" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="1">
-        <v>6</v>
+      <c r="E30" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F30" s="8">
+        <v>0</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
+        <f t="shared" si="2"/>
+        <v>7</v>
       </c>
       <c r="B31" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" s="1">
-        <v>7</v>
+      <c r="E31" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G31" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A32" s="5">
+        <f t="shared" si="2"/>
+        <v>8</v>
       </c>
       <c r="B32" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="1">
-        <v>8</v>
+      <c r="E32" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G32" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A33" s="5">
+        <f t="shared" si="2"/>
+        <v>9</v>
       </c>
       <c r="B33" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" s="1">
-        <v>9</v>
+      <c r="E33" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G33" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A34" s="5">
+        <f t="shared" si="2"/>
+        <v>10</v>
       </c>
       <c r="B34" t="s">
         <v>22</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1003,7 +1148,7 @@
   <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="A30" sqref="A30:A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1497,127 +1642,266 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="5"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="6"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+    </row>
+    <row r="29" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B29" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E29" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>1</v>
+        <f>A29+1</f>
+        <v>2</v>
       </c>
       <c r="B30" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="1">
-        <v>2</v>
+      <c r="E30" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
+        <f t="shared" ref="A31:A42" si="2">A30+1</f>
+        <v>3</v>
       </c>
       <c r="B31" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" s="1">
-        <v>3</v>
+      <c r="E31" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A32" s="5">
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
       <c r="B32" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="1">
-        <v>4</v>
+      <c r="E32" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A33" s="5">
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="B33" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" s="1">
-        <v>5</v>
+      <c r="E33" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G33" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A34" s="5">
+        <f t="shared" si="2"/>
+        <v>6</v>
       </c>
       <c r="B34" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" s="1">
-        <v>6</v>
+      <c r="E34" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A35" s="5">
+        <f t="shared" si="2"/>
+        <v>7</v>
       </c>
       <c r="B35" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" s="1">
-        <v>7</v>
+      <c r="E35" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F35" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G35" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A36" s="5">
+        <f t="shared" si="2"/>
+        <v>8</v>
       </c>
       <c r="B36" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" s="1">
-        <v>8</v>
+      <c r="E36" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A37" s="5">
+        <f t="shared" si="2"/>
+        <v>9</v>
       </c>
       <c r="B37" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" s="1">
-        <v>9</v>
+      <c r="E37" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G37" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A38" s="5">
+        <f t="shared" si="2"/>
+        <v>10</v>
       </c>
       <c r="B38" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" s="1">
-        <v>10</v>
+      <c r="E38" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G38" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A39" s="5">
+        <f t="shared" si="2"/>
+        <v>11</v>
       </c>
       <c r="B39" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" s="1">
-        <v>11</v>
+      <c r="E39" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F39" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G39" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A40" s="5">
+        <f t="shared" si="2"/>
+        <v>12</v>
       </c>
       <c r="B40" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" s="1">
-        <v>12</v>
+      <c r="E40" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F40" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G40" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A41" s="5">
+        <f t="shared" si="2"/>
+        <v>13</v>
       </c>
       <c r="B41" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" s="1">
-        <v>13</v>
+      <c r="E41" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G41" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A42" s="5">
+        <f t="shared" si="2"/>
+        <v>14</v>
       </c>
       <c r="B42" t="s">
         <v>22</v>
+      </c>
+      <c r="E42" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F42" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G42" s="8" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1632,4 +1916,1200 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G62"/>
+  <sheetViews>
+    <sheetView topLeftCell="A18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="32.85546875" customWidth="1"/>
+    <col min="3" max="3" width="38.5703125" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="5">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2">
+        <f>A2</f>
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
+        <f>A2+1</f>
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <f>E2+1</f>
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
+        <f t="shared" ref="A4:A37" si="0">A3+1</f>
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4:E37" si="1">E3+1</f>
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="5">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="5">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G8" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="5">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="F9">
+        <f>F4+1</f>
+        <v>3</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="5">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="F10">
+        <f>F9+1</f>
+        <v>4</v>
+      </c>
+      <c r="G10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="5">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="F11">
+        <f t="shared" ref="F11:F37" si="2">F10+1</f>
+        <v>5</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="F12" s="3">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="G12" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="3">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="F13" s="3">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="G13" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="F14" s="3">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="G14" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" s="3">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="F15" s="3">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="G15" s="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="3">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="F16" s="3">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="G16" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="5">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="G17">
+        <f>G16+1</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="5">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="G18">
+        <f t="shared" ref="G18:G25" si="3">G17+1</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="5">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="5">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>33</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="5">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>34</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="5">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="5">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="5">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>36</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="5">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>37</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="3"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26" s="5">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>17</v>
+      </c>
+      <c r="E26" s="3">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="F26" s="3">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="G26" s="4">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A27" s="5">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>52</v>
+      </c>
+      <c r="E27" s="3">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="F27" s="3">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="G27" s="4">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="5">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>53</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="G28" s="2">
+        <f>G27+1</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="5">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>54</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="G29" s="2">
+        <f t="shared" ref="G29:G36" si="4">G28+1</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="5">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>56</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="G30" s="2">
+        <f t="shared" si="4"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" s="5">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>57</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="G31" s="2">
+        <f t="shared" si="4"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" s="5">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>58</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="G32" s="2">
+        <f t="shared" si="4"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" s="5">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>55</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="G33" s="2">
+        <f t="shared" si="4"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" s="5">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>59</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="G34" s="2">
+        <f t="shared" si="4"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" s="5">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>51</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="2"/>
+        <v>29</v>
+      </c>
+      <c r="G35" s="2">
+        <f t="shared" si="4"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" s="5">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
+        <v>50</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="G36" s="2">
+        <f t="shared" si="4"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A37" s="5">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>49</v>
+      </c>
+      <c r="E37" s="3">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="F37" s="3">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
+      <c r="G37" s="4">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" s="6"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+    </row>
+    <row r="41" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A41" s="5">
+        <v>1</v>
+      </c>
+      <c r="B41" t="s">
+        <v>13</v>
+      </c>
+      <c r="C41" s="5"/>
+      <c r="E41" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G41" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A42" s="5">
+        <f>A41+1</f>
+        <v>2</v>
+      </c>
+      <c r="B42" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42" s="5"/>
+      <c r="E42" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F42" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G42" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A43" s="5">
+        <f t="shared" ref="A43:A62" si="5">A42+1</f>
+        <v>3</v>
+      </c>
+      <c r="B43" t="s">
+        <v>15</v>
+      </c>
+      <c r="C43" s="5"/>
+      <c r="E43" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F43" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G43" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A44" s="5">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="B44" t="s">
+        <v>32</v>
+      </c>
+      <c r="E44" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G44" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A45" s="5">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="B45" t="s">
+        <v>33</v>
+      </c>
+      <c r="E45" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F45" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G45" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A46" s="5">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="B46" t="s">
+        <v>34</v>
+      </c>
+      <c r="E46" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F46" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G46" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A47" s="5">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="B47" t="s">
+        <v>16</v>
+      </c>
+      <c r="C47" s="5"/>
+      <c r="E47" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F47" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G47" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A48" s="5">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="B48" t="s">
+        <v>35</v>
+      </c>
+      <c r="E48" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F48" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G48" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A49" s="5">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="B49" t="s">
+        <v>36</v>
+      </c>
+      <c r="E49" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F49" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G49" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A50" s="5">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="B50" t="s">
+        <v>37</v>
+      </c>
+      <c r="E50" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F50" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G50" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A51" s="5">
+        <f t="shared" si="5"/>
+        <v>11</v>
+      </c>
+      <c r="B51" t="s">
+        <v>17</v>
+      </c>
+      <c r="E51" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F51" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G51" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A52" s="5">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="B52" t="s">
+        <v>18</v>
+      </c>
+      <c r="E52" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F52" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G52" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A53" s="5">
+        <f t="shared" si="5"/>
+        <v>13</v>
+      </c>
+      <c r="B53" t="s">
+        <v>19</v>
+      </c>
+      <c r="E53" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F53" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G53" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A54" s="5">
+        <f t="shared" si="5"/>
+        <v>14</v>
+      </c>
+      <c r="B54" t="s">
+        <v>20</v>
+      </c>
+      <c r="E54" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F54" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G54" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A55" s="5">
+        <f t="shared" si="5"/>
+        <v>15</v>
+      </c>
+      <c r="B55" t="s">
+        <v>21</v>
+      </c>
+      <c r="E55" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F55" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G55" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A56" s="5">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+      <c r="B56" t="s">
+        <v>38</v>
+      </c>
+      <c r="E56" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F56" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G56" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A57" s="5">
+        <f t="shared" si="5"/>
+        <v>17</v>
+      </c>
+      <c r="B57" t="s">
+        <v>39</v>
+      </c>
+      <c r="E57" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F57" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G57" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A58" s="5">
+        <f t="shared" si="5"/>
+        <v>18</v>
+      </c>
+      <c r="B58" t="s">
+        <v>40</v>
+      </c>
+      <c r="E58" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F58" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G58" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A59" s="5">
+        <f t="shared" si="5"/>
+        <v>19</v>
+      </c>
+      <c r="B59" t="s">
+        <v>41</v>
+      </c>
+      <c r="E59" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F59" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G59" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A60" s="5">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="B60" t="s">
+        <v>42</v>
+      </c>
+      <c r="E60" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F60" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G60" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A61" s="5">
+        <f t="shared" si="5"/>
+        <v>21</v>
+      </c>
+      <c r="B61" t="s">
+        <v>43</v>
+      </c>
+      <c r="E61" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F61" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G61" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A62" s="5">
+        <f t="shared" si="5"/>
+        <v>22</v>
+      </c>
+      <c r="B62" t="s">
+        <v>22</v>
+      </c>
+      <c r="E62" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F62" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G62" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="A40:C40"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>